<commit_message>
Added Job Location to spreadsheet and readme
</commit_message>
<xml_diff>
--- a/JobHunt2019.xlsx
+++ b/JobHunt2019.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="254" documentId="11_F25DC773A252ABEACE02EC98EB5D537C5ADE589C" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{43DD5839-27A1-4561-98E1-425509255D4C}"/>
+  <xr:revisionPtr revIDLastSave="257" documentId="11_F25DC773A252ABEACE02EC98EB5D537C5ADE589C" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{AF510FEB-30D5-4C89-BC3B-0FCC90BB41A0}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="100">
   <si>
     <t>Company</t>
   </si>
@@ -315,6 +315,12 @@
   </si>
   <si>
     <t>tst.nointerview</t>
+  </si>
+  <si>
+    <t>JobLocation</t>
+  </si>
+  <si>
+    <t>Denver, CO</t>
   </si>
 </sst>
 </file>
@@ -671,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,15 +691,16 @@
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -713,25 +720,28 @@
         <v>2</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>43620</v>
       </c>
@@ -750,14 +760,17 @@
       <c r="F2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="3"/>
+      <c r="G2" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2" s="3"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="2"/>
       <c r="C3" s="3"/>
@@ -770,8 +783,9 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" s="3"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="2"/>
       <c r="C4" s="3"/>
@@ -784,8 +798,9 @@
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" s="3"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>57</v>
       </c>
@@ -801,62 +816,63 @@
       <c r="F6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="1"/>
+      <c r="H6" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>15</v>
       </c>
       <c r="F7" t="s">
         <v>19</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>27</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>34</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="L7" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>32</v>
       </c>
       <c r="F8" t="s">
         <v>20</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>36</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>37</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>33</v>
       </c>
       <c r="F9" t="s">
         <v>16</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>14</v>
       </c>
@@ -864,7 +880,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>29</v>
       </c>
@@ -872,17 +888,17 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>39</v>
       </c>
@@ -901,7 +917,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C298CAA-2721-4446-B09B-3233B219F044}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>